<commit_message>
Updated Product Backlog and Sprint Backlog
I removed my edited Product Backlog and added back the one from class.
I updated the hours on the sprint backlog to be more realistic.
</commit_message>
<xml_diff>
--- a/documentation/Sprint Backlog  Burndown.xlsx
+++ b/documentation/Sprint Backlog  Burndown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pikac\Desktop\Software Engineering\GroupPirateShipInventory\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0854baf48ed3e786/Documents/College Docs/Software Engineering/Round 2/Projects/Project 2/GroupPirateShipInventory/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025DB07E-3CC9-4A6A-8309-1B249045E885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{025DB07E-3CC9-4A6A-8309-1B249045E885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E71FD38E-7AF3-48C0-93E9-7333F965DAFC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="2424" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18756" yWindow="17172" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -297,12 +297,6 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -314,6 +308,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -323,18 +326,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,7 +449,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1506,372 +1506,372 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.44140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="57.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="47.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="4" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <v>6</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-    </row>
-    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="5" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>3</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="6" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="6" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15"/>
+      <c r="B7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="10">
         <v>1</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="12"/>
-      <c r="B7" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="15">
-        <v>1</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-    </row>
-    <row r="8" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="12">
         <v>4</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="13">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="12"/>
-      <c r="B10" s="15" t="s">
+      <c r="D9" s="8">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15"/>
+      <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="10">
         <v>2</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="8" t="s">
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9">
+      <c r="C27" s="6"/>
+      <c r="D27" s="7">
         <f>SUM(D3:D26)</f>
-        <v>19</v>
-      </c>
-      <c r="E27" s="9">
+        <v>21</v>
+      </c>
+      <c r="E27" s="7">
         <f t="shared" ref="E27:H27" si="0">SUM(E3:E26)</f>
         <v>0</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>

</xml_diff>